<commit_message>
updates, readmes, minor fixes
</commit_message>
<xml_diff>
--- a/tools/samples/adhoc-prep.xlsx
+++ b/tools/samples/adhoc-prep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airah/Desktop/WCC/wcc/tools/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C46AEB7-A598-7145-A23E-8074A5220FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412FBB1-9422-4440-A810-C111116B0320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="27200" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Mentor Name</t>
   </si>
@@ -28,43 +28,10 @@
     <t>Availability (Hours)</t>
   </si>
   <si>
-    <t>Madhura Chaganty</t>
+    <t>Mentor1 Surname</t>
   </si>
   <si>
-    <t>Ana Nogal</t>
-  </si>
-  <si>
-    <t>Rajani Rao</t>
-  </si>
-  <si>
-    <t>Sonali Goel</t>
-  </si>
-  <si>
-    <t>Samuela Smolorz</t>
-  </si>
-  <si>
-    <t>Dan Antonela</t>
-  </si>
-  <si>
-    <t>Gabriel Oliveira</t>
-  </si>
-  <si>
-    <t>Bryan Boreham</t>
-  </si>
-  <si>
-    <t>Sonika Janagill</t>
-  </si>
-  <si>
-    <t>Arzu Guney Caner</t>
-  </si>
-  <si>
-    <t>Eleonora Belova</t>
-  </si>
-  <si>
-    <t>Adriana Zencke Zimmermann</t>
-  </si>
-  <si>
-    <t>Andrew King</t>
+    <t>Mentor2 Surname</t>
   </si>
 </sst>
 </file>
@@ -463,11 +430,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BR14"/>
+  <dimension ref="A1:BR17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -587,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE2" s="5"/>
     </row>
@@ -596,96 +563,50 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
+      <c r="A4" s="9"/>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
+      <c r="A5" s="9"/>
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
+      <c r="A6" s="9"/>
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
+      <c r="A7" s="9"/>
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
+      <c r="A8" s="9"/>
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
+      <c r="A9" s="9"/>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
+      <c r="A10" s="9"/>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
+      <c r="A11" s="9"/>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
+      <c r="A12" s="9"/>
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
+      <c r="A13" s="8"/>
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>